<commit_message>
Correct sail number in Excel results
</commit_message>
<xml_diff>
--- a/events/2025/sailwave/iswc-results-2025.xlsx
+++ b/events/2025/sailwave/iswc-results-2025.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mwgeo\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\mike\projects\work\wst-results\events\2025\sailwave\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BDA1CE8C-9993-4C6F-8D29-0BBE6D9D1545}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C01F7D-AF04-484B-A1AA-2CDF82E6B247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="23236" windowHeight="13875" xr2:uid="{AECD1B0A-33E9-4734-866A-4563E9326497}"/>
   </bookViews>
@@ -1017,9 +1017,6 @@
     <t>Maria Natal Ama</t>
   </si>
   <si>
-    <t>FRA-111</t>
-  </si>
-  <si>
     <t>(0.7)</t>
   </si>
   <si>
@@ -1072,6 +1069,9 @@
   </si>
   <si>
     <t>(10.0)</t>
+  </si>
+  <si>
+    <t>POR-111</t>
   </si>
 </sst>
 </file>
@@ -1522,16 +1522,16 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>330</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>331</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>2</v>
@@ -3228,16 +3228,16 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>330</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>331</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>2</v>
@@ -3370,7 +3370,7 @@
         <v>324</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>325</v>
+        <v>343</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>14</v>
@@ -3424,16 +3424,16 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>330</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>331</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>2</v>
@@ -3453,7 +3453,7 @@
         <v>34</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>124</v>
@@ -3482,7 +3482,7 @@
         <v>72</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="E3" s="7" t="s">
         <v>122</v>
@@ -3591,16 +3591,16 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>330</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>331</v>
       </c>
       <c r="H1" s="6" t="s">
         <v>2</v>
@@ -3620,7 +3620,7 @@
         <v>9</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E2" s="7" t="s">
         <v>124</v>
@@ -3678,7 +3678,7 @@
         <v>78</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E4" s="7" t="s">
         <v>128</v>
@@ -3730,10 +3730,10 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>332</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>333</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>334</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>14</v>
@@ -3759,10 +3759,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
+        <v>334</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>335</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>336</v>
       </c>
       <c r="D7" s="7" t="s">
         <v>14</v>
@@ -3818,22 +3818,22 @@
         <v>1</v>
       </c>
       <c r="D1" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>328</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="G1" s="6" t="s">
-        <v>331</v>
-      </c>
       <c r="H1" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>338</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>339</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>2</v>
@@ -3894,7 +3894,7 @@
         <v>128</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="G3" s="7" t="s">
         <v>145</v>
@@ -4037,7 +4037,7 @@
         <v>139</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>134</v>
@@ -4066,7 +4066,7 @@
         <v>122</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>130</v>
@@ -4107,7 +4107,7 @@
         <v>144</v>
       </c>
       <c r="G9" s="7" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>144</v>
@@ -4139,7 +4139,7 @@
         <v>149</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="G10" s="7" t="s">
         <v>144</v>
@@ -4206,7 +4206,7 @@
         <v>14</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="F12" s="7" t="s">
         <v>149</v>
@@ -4687,10 +4687,10 @@
         <v>13</v>
       </c>
       <c r="B26" t="s">
+        <v>334</v>
+      </c>
+      <c r="C26" s="8" t="s">
         <v>335</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>336</v>
       </c>
       <c r="D26" s="7" t="s">
         <v>14</v>

</xml_diff>